<commit_message>
Database wilayah Indonesia 2018 Semester 1
</commit_message>
<xml_diff>
--- a/Import/BPS Province.xlsx
+++ b/Import/BPS Province.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laragon\Lokasi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laragon\Lokasi\Import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638272D5-5253-4220-8145-C2CC2A434CA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A29EFE5C-4A64-4ED1-BD1F-01C8EA4483B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13290" xr2:uid="{AE6E2D77-2118-453C-9076-A00D10193B54}"/>
   </bookViews>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
-    <t>bps_name</t>
-  </si>
-  <si>
     <t>ACEH</t>
   </si>
   <si>
@@ -133,6 +130,9 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
 </sst>
 </file>
@@ -550,8 +550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A10FBE11-CA96-44A9-A7DE-4A1D38FA7EED}">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,10 +563,10 @@
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -574,7 +574,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -582,7 +582,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -590,7 +590,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -598,7 +598,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -606,7 +606,7 @@
         <v>15</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -614,7 +614,7 @@
         <v>16</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -622,7 +622,7 @@
         <v>17</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -630,7 +630,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -638,7 +638,7 @@
         <v>19</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -646,7 +646,7 @@
         <v>21</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -654,7 +654,7 @@
         <v>31</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -662,7 +662,7 @@
         <v>32</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -670,7 +670,7 @@
         <v>33</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -678,7 +678,7 @@
         <v>34</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -686,7 +686,7 @@
         <v>35</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -694,7 +694,7 @@
         <v>36</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -702,7 +702,7 @@
         <v>51</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -710,7 +710,7 @@
         <v>52</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -718,7 +718,7 @@
         <v>53</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -726,7 +726,7 @@
         <v>61</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -734,7 +734,7 @@
         <v>62</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -742,7 +742,7 @@
         <v>63</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -750,7 +750,7 @@
         <v>64</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -758,7 +758,7 @@
         <v>65</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -766,7 +766,7 @@
         <v>71</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -774,7 +774,7 @@
         <v>72</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -782,7 +782,7 @@
         <v>73</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -790,7 +790,7 @@
         <v>74</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -798,7 +798,7 @@
         <v>75</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -806,7 +806,7 @@
         <v>76</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -814,7 +814,7 @@
         <v>81</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -822,7 +822,7 @@
         <v>82</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -830,7 +830,7 @@
         <v>91</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -838,7 +838,7 @@
         <v>94</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>